<commit_message>
Added equipment options to Silberhelme
</commit_message>
<xml_diff>
--- a/resources/db/EquipmentOptions.xlsx
+++ b/resources/db/EquipmentOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B91D7B-41DB-4610-B50E-28C47E81C9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A267BE-8B60-44E2-A69B-C0F77391E183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,11 +482,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E713F92B-F931-47AC-9A06-8B605BE422D6}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>